<commit_message>
EPBDS-2847 Generate custom typed SpreadsheetResult. Added possibility to test spreadsheet cells via test table.
</commit_message>
<xml_diff>
--- a/DEV/trunk/org.openl.rules/test/rules/calc1/ArrayInSpreadsheet.xlsx
+++ b/DEV/trunk/org.openl.rules/test/rules/calc1/ArrayInSpreadsheet.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="120" windowWidth="24915" windowHeight="12075"/>
+    <workbookView xWindow="120" yWindow="120" windowWidth="24915" windowHeight="12075" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Лист1" sheetId="1" r:id="rId1"/>
-    <sheet name="Лист2" sheetId="2" r:id="rId2"/>
+    <sheet name="Test Datatype Array" sheetId="1" r:id="rId1"/>
+    <sheet name="Test Array" sheetId="2" r:id="rId2"/>
     <sheet name="Лист3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="30">
   <si>
     <t>Value</t>
   </si>
@@ -88,12 +88,37 @@
 income.drivers = drivers;
 return drivers;</t>
   </si>
+  <si>
+    <t xml:space="preserve">Spreadsheet DoubleValue[] testDoubleValue()
+</t>
+  </si>
+  <si>
+    <t>{getDVs()}</t>
+  </si>
+  <si>
+    <t>return new DoubleValue[]{new DoubleValue(1.23), new DoubleValue(5.24)};</t>
+  </si>
+  <si>
+    <t>Method DoubleValue[] getDVs()</t>
+  </si>
+  <si>
+    <t>DVs : DoubleValue[]</t>
+  </si>
+  <si>
+    <t>=$DVs</t>
+  </si>
+  <si>
+    <t>AnyValue</t>
+  </si>
+  <si>
+    <t>= 78</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="6">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -227,7 +252,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="3" xfId="2" applyBorder="1"/>
@@ -240,6 +265,7 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="1" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -260,6 +286,16 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="1" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -269,6 +305,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -347,6 +388,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -381,6 +423,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Стандартная">
@@ -556,14 +599,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C2:M16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C7" sqref="C7:E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="60.42578125" customWidth="1"/>
     <col min="5" max="5" width="17" customWidth="1"/>
@@ -571,48 +614,48 @@
     <col min="13" max="13" width="11.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:13">
+    <row r="2" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C2" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="3:13">
+    <row r="3" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C3" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="3:13">
-      <c r="C7" s="11" t="s">
+    <row r="7" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C7" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="11"/>
-      <c r="E7" s="11"/>
-    </row>
-    <row r="8" spans="3:13">
+      <c r="D7" s="12"/>
+      <c r="E7" s="12"/>
+    </row>
+    <row r="8" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C8" s="4"/>
-      <c r="D8" s="12" t="s">
+      <c r="D8" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="E8" s="12"/>
-    </row>
-    <row r="9" spans="3:13">
+      <c r="E8" s="13"/>
+    </row>
+    <row r="9" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C9" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D9" s="13" t="s">
+      <c r="D9" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="E9" s="14"/>
-      <c r="I9" s="8" t="s">
+      <c r="E9" s="15"/>
+      <c r="I9" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="J9" s="8"/>
-      <c r="L9" s="8" t="s">
+      <c r="J9" s="9"/>
+      <c r="L9" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="M9" s="8"/>
-    </row>
-    <row r="10" spans="3:13">
+      <c r="M9" s="9"/>
+    </row>
+    <row r="10" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C10" s="1" t="s">
         <v>15</v>
       </c>
@@ -633,14 +676,14 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="3:13">
+    <row r="11" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C11" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D11" s="9" t="s">
+      <c r="D11" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="E11" s="10"/>
+      <c r="E11" s="11"/>
       <c r="I11" s="1" t="s">
         <v>3</v>
       </c>
@@ -654,7 +697,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="3:13">
+    <row r="12" spans="3:13" x14ac:dyDescent="0.25">
       <c r="I12" s="1" t="s">
         <v>6</v>
       </c>
@@ -662,12 +705,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="3:13">
+    <row r="15" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C15" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="16" spans="3:13" ht="75">
+    <row r="16" spans="3:13" ht="75" x14ac:dyDescent="0.25">
       <c r="C16" s="3" t="s">
         <v>21</v>
       </c>
@@ -687,24 +730,86 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="C5:I9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="16.85546875" customWidth="1"/>
+    <col min="5" max="5" width="34" customWidth="1"/>
+    <col min="9" max="9" width="70.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="5" spans="3:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C5" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" s="12"/>
+      <c r="E5" s="12"/>
+      <c r="I5" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C6" s="4"/>
+      <c r="D6" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="E6" s="13"/>
+      <c r="I6" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C7" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="E7" s="16"/>
+      <c r="I7" s="17"/>
+    </row>
+    <row r="8" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C8" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="E8" s="7"/>
+    </row>
+    <row r="9" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C9" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D9" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="E9" s="11"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="C5:E5"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="D9:E9"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>